<commit_message>
Updated 10 channels calculations
</commit_message>
<xml_diff>
--- a/VSC/Calcul10.xlsx
+++ b/VSC/Calcul10.xlsx
@@ -25,19 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>9 kanalen</t>
   </si>
   <si>
     <t>10 kanalen</t>
   </si>
+  <si>
+    <t>8 kanalen</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>GOK 9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,13 +83,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Procent" xfId="2" builtinId="5"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -138,7 +172,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$B$1</c:f>
+              <c:f>Blad1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -269,9 +303,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$B$2:$B$26</c:f>
+              <c:f>Blad1!$C$2:$C$26</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -358,7 +392,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blad1!$C$1</c:f>
+              <c:f>Blad1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -489,10 +523,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad1!$C$2:$C$30</c:f>
+              <c:f>Blad1!$F$2:$F$30</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>3.0</c:v>
                 </c:pt>
@@ -522,6 +559,57 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>544888.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.26276811758196E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.24292073821933E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.55548403289389E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.05067347942625E7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.67731272599546E7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.33198230517593E6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.94499484369431E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.33198677322926E6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>362410.9064667728</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>86727.38576426282</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24152.29862512842</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8688.77705273278</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3959.28614563471</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1445.308129703535</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>222.5808471592981</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>1.0</c:v>
@@ -616,7 +704,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1567,317 +1655,1279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="E3">
-        <f>C3/B3</f>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <f>F3/C3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>7</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E26" si="0">C4/B4</f>
+      <c r="D4" s="3">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <f>B4/B3</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="K4">
+        <f>C4/C3</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O12" si="0">F4/C4</f>
         <v>1</v>
       </c>
+      <c r="Q4">
+        <f>C4/C3</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="T4">
+        <f>F4/F3</f>
+        <v>2.3333333333333335</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>20</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="D5" s="3">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H20" si="1">B5/B4</f>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="I5">
+        <f>H5/H4</f>
+        <v>1.2244897959183674</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K11" si="2">C5/C4</f>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="L5">
+        <f>K5/K4</f>
+        <v>1.2244897959183674</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q26" si="3">C5/C4</f>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="R5">
+        <f>Q5/Q4</f>
+        <v>1.2244897959183674</v>
+      </c>
+      <c r="T5">
+        <f>F5/F4</f>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="U5">
+        <f>T5/T4</f>
+        <v>1.2244897959183674</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <v>57</v>
+      </c>
+      <c r="C6" s="3">
         <v>59</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="3">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
         <v>60</v>
       </c>
-      <c r="E6">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I20" si="4">H6/H5</f>
+        <v>0.99750000000000005</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>2.95</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L10" si="5">K6/K5</f>
+        <v>1.0325</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="0"/>
         <v>1.0169491525423728</v>
       </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>2.95</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:R26" si="6">Q6/Q5</f>
+        <v>1.0325</v>
+      </c>
+      <c r="T6">
+        <f>F6/F5</f>
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ref="U6:U12" si="7">T6/T5</f>
+        <v>1.05</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
+        <v>189</v>
+      </c>
+      <c r="C7" s="3">
         <v>208</v>
       </c>
-      <c r="C7">
+      <c r="D7" s="3">
+        <v>208</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <v>214</v>
       </c>
-      <c r="E7">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>3.3157894736842106</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>1.1634349030470914</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>3.5254237288135593</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="5"/>
+        <v>1.1950588911232403</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="0"/>
         <v>1.0288461538461537</v>
       </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>3.5254237288135593</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="6"/>
+        <v>1.1950588911232403</v>
+      </c>
+      <c r="T7">
+        <f>F7/F6</f>
+        <v>3.5666666666666669</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="7"/>
+        <v>1.1888888888888889</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
+        <v>648</v>
+      </c>
+      <c r="C8" s="3">
         <v>807</v>
       </c>
-      <c r="C8">
+      <c r="D8" s="3">
+        <v>807</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
         <v>864</v>
       </c>
-      <c r="E8">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>1.0340136054421767</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>3.8798076923076925</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="5"/>
+        <v>1.1005223742603552</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="0"/>
         <v>1.0706319702602229</v>
       </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>3.8798076923076925</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="6"/>
+        <v>1.1005223742603552</v>
+      </c>
+      <c r="T8">
+        <f>F8/F7</f>
+        <v>4.037383177570093</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="7"/>
+        <v>1.1319765918420821</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
+        <v>2088</v>
+      </c>
+      <c r="C9" s="3">
         <v>3415</v>
       </c>
-      <c r="C9">
+      <c r="D9" s="3">
+        <v>3415</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
         <v>3996</v>
       </c>
-      <c r="E9">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>3.2222222222222223</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>0.93981481481481488</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>4.2317224287484514</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="5"/>
+        <v>1.0907041699872093</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="0"/>
         <v>1.1701317715959005</v>
       </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>4.2317224287484514</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="6"/>
+        <v>1.0907041699872093</v>
+      </c>
+      <c r="T9">
+        <f>F9/F8</f>
+        <v>4.625</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="7"/>
+        <v>1.1455439814814816</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
+        <v>5702</v>
+      </c>
+      <c r="C10" s="3">
         <v>14340</v>
       </c>
-      <c r="C10">
+      <c r="D10" s="3">
+        <v>14340</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
         <v>20125</v>
       </c>
-      <c r="E10">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2.7308429118773945</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>0.84750297265160512</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>4.1991215226939973</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="5"/>
+        <v>0.99229606700265172</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="0"/>
         <v>1.4034170153417016</v>
       </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>4.1991215226939973</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="6"/>
+        <v>0.99229606700265172</v>
+      </c>
+      <c r="T10">
+        <f>F10/F9</f>
+        <v>5.0362862862862867</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="7"/>
+        <v>1.0889267646024403</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
+        <v>11669</v>
+      </c>
+      <c r="C11" s="3">
         <v>55986</v>
       </c>
-      <c r="C11">
+      <c r="D11" s="3">
+        <v>55986</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
         <v>105325</v>
       </c>
-      <c r="E11">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>2.0464749210803226</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>0.74939313139524966</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>3.9041841004184099</v>
+      </c>
+      <c r="L11">
+        <v>0.93981481481481488</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="0"/>
         <v>1.8812738899010466</v>
       </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>3.9041841004184099</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="6"/>
+        <v>0.92976211317495605</v>
+      </c>
+      <c r="T11">
+        <f>F11/F10</f>
+        <v>5.2335403726708076</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="7"/>
+        <v>1.0391665753636048</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
+        <v>16108</v>
+      </c>
+      <c r="C12" s="3">
         <v>188710</v>
       </c>
-      <c r="C12">
+      <c r="D12" s="3">
+        <f>D11*K12</f>
+        <v>185246.90402265682</v>
+      </c>
+      <c r="E12" s="4">
+        <f>(C12-D12)/C12</f>
+        <v>1.8351417398882849E-2</v>
+      </c>
+      <c r="F12" s="3">
         <v>544888</v>
       </c>
-      <c r="E12">
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1.3804096323592425</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>0.67453044165844556</v>
+      </c>
+      <c r="K12">
+        <f>K11*L12</f>
+        <v>3.3088076308837353</v>
+      </c>
+      <c r="L12">
+        <v>0.84750297265160512</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="0"/>
         <v>2.8874357479730803</v>
       </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>3.3706640945950772</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="6"/>
+        <v>0.86334660658902951</v>
+      </c>
+      <c r="T12">
+        <f>F12/F11</f>
+        <v>5.1733966294801803</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="7"/>
+        <v>0.98850801963720503</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
+        <v>13345</v>
+      </c>
+      <c r="C13" s="3">
         <v>490288</v>
       </c>
+      <c r="D13" s="3">
+        <f>D12*K13</f>
+        <v>459337.79931269254</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" ref="E13:E24" si="8">(C13-D13)/C13</f>
+        <v>6.3126571907343151E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <f>T14*F12</f>
+        <v>2262768.1175819566</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.82847032530419662</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>0.60016266612705926</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13:K22" si="9">K12*L13</f>
+        <v>2.4795977116924597</v>
+      </c>
+      <c r="L13">
+        <v>0.74939313139524966</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="3"/>
+        <v>2.5981029092257963</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="6"/>
+        <v>0.77079852406292959</v>
+      </c>
+      <c r="T13">
+        <f>T12*U13</f>
+        <v>4.8100281825176872</v>
+      </c>
+      <c r="U13">
+        <v>0.92976211317495605</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
+        <v>6758</v>
+      </c>
+      <c r="C14" s="3">
         <v>854645</v>
       </c>
+      <c r="D14" s="3">
+        <f>D13*K14</f>
+        <v>768271.93109465449</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="8"/>
+        <v>0.10106309509251854</v>
+      </c>
+      <c r="F14" s="3">
+        <f>T15*F13</f>
+        <v>7242920.7382193282</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0.50640689396777816</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>0.61125532019730022</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="9"/>
+        <v>1.6725641396031858</v>
+      </c>
+      <c r="L14">
+        <v>0.67453044165844556</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="3"/>
+        <v>1.7431489247136378</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="6"/>
+        <v>0.67093143944520484</v>
+      </c>
+      <c r="T14">
+        <f t="shared" ref="T14:T28" si="10">T13*U14</f>
+        <v>4.152721508974242</v>
+      </c>
+      <c r="U14">
+        <v>0.86334660658902951</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
+        <v>2269</v>
+      </c>
+      <c r="C15" s="3">
         <v>914533</v>
       </c>
+      <c r="D15" s="3">
+        <f>D14*K15</f>
+        <v>771199.47223142162</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="8"/>
+        <v>0.15672865579326101</v>
+      </c>
+      <c r="F15" s="3">
+        <f>T16*F14</f>
+        <v>15554840.328938868</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.33575022195915949</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>0.66300484049200703</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="9"/>
+        <v>1.003810553292759</v>
+      </c>
+      <c r="L15">
+        <v>0.60016266612705926</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="3"/>
+        <v>1.0700735393057936</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="6"/>
+        <v>0.61387384871982975</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="10"/>
+        <v>3.2009116099617274</v>
+      </c>
+      <c r="U15">
+        <v>0.77079852406292959</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
+        <v>527</v>
+      </c>
+      <c r="C16" s="3">
         <v>607155</v>
       </c>
+      <c r="D16" s="3">
+        <f>D15*K16</f>
+        <v>473196.07431996724</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="8"/>
+        <v>0.22063381785546154</v>
+      </c>
+      <c r="F16" s="3">
+        <f>T17*F15</f>
+        <v>20506734.79426254</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0.23226090788893786</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>0.69176695262822485</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>0.61358454117039452</v>
+      </c>
+      <c r="L16">
+        <v>0.61125532019730022</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="3"/>
+        <v>0.66389621806976895</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="6"/>
+        <v>0.62042111470251782</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="10"/>
+        <v>2.1475922340084899</v>
+      </c>
+      <c r="U16">
+        <v>0.67093143944520484</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
+        <v>81</v>
+      </c>
+      <c r="C17" s="3">
         <v>274184</v>
       </c>
+      <c r="D17" s="3">
+        <f>D16*K17</f>
+        <v>192500.6682608056</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="8"/>
+        <v>0.2979142901817553</v>
+      </c>
+      <c r="F17" s="3">
+        <f>T18*F16</f>
+        <v>16773127.259954559</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0.15370018975332067</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>0.66175660445974305</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>0.40680952084703875</v>
+      </c>
+      <c r="L17">
+        <v>0.66300484049200703</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="3"/>
+        <v>0.45158814470769409</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="6"/>
+        <v>0.68020894292884293</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="10"/>
+        <v>1.318350710171609</v>
+      </c>
+      <c r="U17">
+        <v>0.61387384871982975</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3">
         <v>94080</v>
       </c>
+      <c r="D18" s="3">
+        <f>D17*K18</f>
+        <v>54173.034198483838</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="8"/>
+        <v>0.42418118411475514</v>
+      </c>
+      <c r="F18" s="3">
+        <f>T19*F17</f>
+        <v>9331982.305175934</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0.2839506172839506</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>1.8474317939338516</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>0.28141738253650428</v>
+      </c>
+      <c r="L18">
+        <v>0.69176695262822485</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="3"/>
+        <v>0.34312724301928632</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="6"/>
+        <v>0.75982340776768442</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="10"/>
+        <v>0.81793261717352561</v>
+      </c>
+      <c r="U18">
+        <v>0.62042111470251782</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
         <v>25783</v>
       </c>
+      <c r="D19" s="3">
+        <f>D18*K19</f>
+        <v>10088.633947345777</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="8"/>
+        <v>0.60870984961618979</v>
+      </c>
+      <c r="F19" s="3">
+        <f>T20*F18</f>
+        <v>3944994.8436943125</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>0.91871455576559546</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>0.18622981150330567</v>
+      </c>
+      <c r="L19">
+        <v>0.66175660445974305</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="3"/>
+        <v>0.27405399659863944</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="6"/>
+        <v>0.79869495114159605</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="10"/>
+        <v>0.55636508091462578</v>
+      </c>
+      <c r="U19">
+        <v>0.68020894292884293</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
         <v>5694</v>
       </c>
+      <c r="D20" s="3">
+        <f>D19*K20</f>
+        <v>3470.9629800761777</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="8"/>
+        <v>0.39041746047134218</v>
+      </c>
+      <c r="F20" s="3">
+        <f>T21*F19</f>
+        <v>1331986.7732292558</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="9"/>
+        <v>0.34404687474951501</v>
+      </c>
+      <c r="L20">
+        <v>1.8474317939338516</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="3"/>
+        <v>0.22084319125004848</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="6"/>
+        <v>0.80583824352498012</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="10"/>
+        <v>0.42273921174349444</v>
+      </c>
+      <c r="U20">
+        <v>0.75982340776768442</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1"/>
+      <c r="C21" s="3">
         <v>1106</v>
       </c>
+      <c r="D21" s="3">
+        <f>D20*K21</f>
+        <v>1097.1050043741125</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="8"/>
+        <v>8.0424915243106077E-3</v>
+      </c>
+      <c r="F21" s="3">
+        <f>T22*F20</f>
+        <v>362410.90646677278</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="9"/>
+        <v>0.31608087169804217</v>
+      </c>
+      <c r="L21">
+        <v>0.91871455576559546</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="3"/>
+        <v>0.19423955040393395</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="6"/>
+        <v>0.87953606042582178</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="10"/>
+        <v>0.33763967406910711</v>
+      </c>
+      <c r="U21">
+        <v>0.79869495114159605</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1"/>
+      <c r="C22" s="3">
         <v>250</v>
       </c>
+      <c r="D22" s="3">
+        <f>D21*K22</f>
+        <v>221.54999558104549</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="8"/>
+        <v>0.11380001767581803</v>
+      </c>
+      <c r="F22" s="3">
+        <f>T23*F21</f>
+        <v>86727.385764262828</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="9"/>
+        <v>0.2019405569181936</v>
+      </c>
+      <c r="L22">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="3"/>
+        <v>0.22603978300180833</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="6"/>
+        <v>1.1637165681847168</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="10"/>
+        <v>0.27208296189619607</v>
+      </c>
+      <c r="U22">
+        <v>0.80583824352498012</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1"/>
+      <c r="C23" s="3">
         <v>73</v>
       </c>
+      <c r="D23" s="3">
+        <v>70</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="8"/>
+        <v>4.1095890410958902E-2</v>
+      </c>
+      <c r="F23" s="3">
+        <f>T24*F22</f>
+        <v>24152.29862512842</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="3"/>
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="6"/>
+        <v>1.2918079999999998</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="10"/>
+        <v>0.23930677641516929</v>
+      </c>
+      <c r="U23">
+        <v>0.87953606042582178</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1"/>
+      <c r="C24" s="3">
         <v>27</v>
       </c>
+      <c r="D24" s="3">
+        <v>25</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="8"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <f>T25*F23</f>
+        <v>8688.7770527327812</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="3"/>
+        <v>0.36986301369863012</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="6"/>
+        <v>1.2666541565021581</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="10"/>
+        <v>0.27848526059320811</v>
+      </c>
+      <c r="U24">
+        <v>1.1637165681847168</v>
+      </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="3">
         <v>8</v>
       </c>
+      <c r="D25" s="3">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <f>T26*F24</f>
+        <v>3959.2861456347105</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="3"/>
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="6"/>
+        <v>0.80109739368998634</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="10"/>
+        <v>0.35974948751639091</v>
+      </c>
+      <c r="U25">
+        <v>1.2918079999999998</v>
+      </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1"/>
+      <c r="C26" s="3">
         <v>1</v>
       </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <f>T27*F25</f>
+        <v>1445.3081297035353</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="6"/>
+        <v>0.421875</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="10"/>
+        <v>0.45567818366215779</v>
+      </c>
+      <c r="U26">
+        <v>1.2666541565021581</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" s="1"/>
+      <c r="F27" s="3">
+        <f>T28*F26</f>
+        <v>222.58084715929812</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="10"/>
+        <v>0.36504260529314153</v>
+      </c>
+      <c r="U27">
+        <v>0.80109739368998634</v>
+      </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" s="1"/>
+      <c r="F28" s="3">
+        <v>50</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="10"/>
+        <v>0.15400234910804408</v>
+      </c>
+      <c r="U28">
+        <v>0.421875</v>
+      </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" s="1"/>
+      <c r="F29" s="3">
+        <v>29</v>
+      </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="1"/>
+      <c r="F30" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B26">
+  <conditionalFormatting sqref="C2:C26">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F30">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E6 D7:D26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Removed empty Error files from VSC
</commit_message>
<xml_diff>
--- a/VSC/Calcul10.xlsx
+++ b/VSC/Calcul10.xlsx
@@ -1658,13 +1658,13 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9" style="2" customWidth="1"/>
+    <col min="4" max="5" width="9" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Some addings to the excel files
</commit_message>
<xml_diff>
--- a/VSC/Calcul10.xlsx
+++ b/VSC/Calcul10.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="14540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Grafiek1" sheetId="2" r:id="rId1"/>
     <sheet name="Blad1" sheetId="1" r:id="rId2"/>
+    <sheet name="Grafiek2" sheetId="4" r:id="rId3"/>
+    <sheet name="Blad2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -48,7 +50,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -88,18 +90,21 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -561,49 +566,49 @@
                   <c:v>544888.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.26276811758196E6</c:v>
+                  <c:v>2.624951E6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.24292073821933E6</c:v>
+                  <c:v>8.40223613148065E6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.55548403289389E7</c:v>
+                  <c:v>1.80445770642734E7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.05067347942625E7</c:v>
+                  <c:v>2.37890809874311E7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.67731272599546E7</c:v>
+                  <c:v>1.94578652722025E7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.33198230517593E6</c:v>
+                  <c:v>1.08256767865948E7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.94499484369431E6</c:v>
+                  <c:v>4.57643807135495E6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.33198677322926E6</c:v>
+                  <c:v>1.54518705880974E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>362410.9064667728</c:v>
+                  <c:v>420419.0716446248</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>86727.38576426282</c:v>
+                  <c:v>100609.1327787333</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24152.29862512842</c:v>
+                  <c:v>28018.16055994221</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8688.77705273278</c:v>
+                  <c:v>10079.51890259117</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3959.28614563471</c:v>
+                  <c:v>4593.016865721128</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1445.308129703535</c:v>
+                  <c:v>1676.64684281818</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>222.5808471592981</c:v>
+                  <c:v>258.2075524185853</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>50.0</c:v>
@@ -629,11 +634,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114193472"/>
-        <c:axId val="-2114175312"/>
+        <c:axId val="-2144993632"/>
+        <c:axId val="2121896256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114193472"/>
+        <c:axId val="-2144993632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +681,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114175312"/>
+        <c:crossAx val="2121896256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -684,7 +689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114175312"/>
+        <c:axId val="2121896256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +740,487 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114193472"/>
+        <c:crossAx val="-2144993632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-BE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$A$1:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad2!$B$1:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>245.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1669.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15624.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>154239.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.062174E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.797288E6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.661054E6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.404493E6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>898401.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>126276.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12442.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>976.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2144763872"/>
+        <c:axId val="-2145002480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2144763872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2145002480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2145002480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2144763872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -851,6 +1336,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1354,11 +1879,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1366,6 +2405,33 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9321101" cy="6082018"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -1655,20 +2721,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A2" zoomScale="89" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="2" customWidth="1"/>
+    <col min="6" max="9" width="12.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -1682,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1697,8 +2763,11 @@
       <c r="F2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1715,12 +2784,15 @@
       <c r="F3" s="3">
         <v>3</v>
       </c>
-      <c r="O3">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="R3">
         <f>F3/C3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1737,28 +2809,31 @@
       <c r="F4" s="3">
         <v>7</v>
       </c>
-      <c r="H4">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4">
         <f>B4/B3</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <f>C4/C3</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="O4">
-        <f t="shared" ref="O4:O12" si="0">F4/C4</f>
+      <c r="R4">
+        <f t="shared" ref="R4:R12" si="0">F4/C4</f>
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <f>C4/C3</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="T4">
-        <f>F4/F3</f>
+      <c r="W4">
+        <f t="shared" ref="W4:W12" si="1">F4/F3</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1775,44 +2850,47 @@
       <c r="F5" s="3">
         <v>20</v>
       </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H20" si="1">B5/B4</f>
-        <v>2.8571428571428572</v>
-      </c>
-      <c r="I5">
-        <f>H5/H4</f>
-        <v>1.2244897959183674</v>
-      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="K5">
-        <f t="shared" ref="K5:K11" si="2">C5/C4</f>
+        <f t="shared" ref="K5:K20" si="2">B5/B4</f>
         <v>2.8571428571428572</v>
       </c>
       <c r="L5">
         <f>K5/K4</f>
         <v>1.2244897959183674</v>
       </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N11" si="3">C5/C4</f>
+        <v>2.8571428571428572</v>
+      </c>
       <c r="O5">
+        <f>N5/N4</f>
+        <v>1.2244897959183674</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q5">
-        <f t="shared" ref="Q5:Q26" si="3">C5/C4</f>
-        <v>2.8571428571428572</v>
-      </c>
-      <c r="R5">
-        <f>Q5/Q4</f>
-        <v>1.2244897959183674</v>
-      </c>
       <c r="T5">
-        <f>F5/F4</f>
+        <f t="shared" ref="T5:T26" si="4">C5/C4</f>
         <v>2.8571428571428572</v>
       </c>
       <c r="U5">
         <f>T5/T4</f>
         <v>1.2244897959183674</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W5">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="X5">
+        <f>W5/W4</f>
+        <v>1.2244897959183674</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1829,44 +2907,47 @@
       <c r="F6" s="3">
         <v>60</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>2.85</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I20" si="4">H6/H5</f>
-        <v>0.99750000000000005</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
       <c r="K6">
         <f t="shared" si="2"/>
+        <v>2.85</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L20" si="5">K6/K5</f>
+        <v>0.99750000000000005</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
         <v>2.95</v>
       </c>
-      <c r="L6">
-        <f t="shared" ref="L6:L10" si="5">K6/K5</f>
+      <c r="O6">
+        <f t="shared" ref="O6:O10" si="6">N6/N5</f>
         <v>1.0325</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <f t="shared" si="0"/>
         <v>1.0169491525423728</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
+      <c r="T6">
+        <f t="shared" si="4"/>
         <v>2.95</v>
       </c>
-      <c r="R6">
-        <f t="shared" ref="R6:R26" si="6">Q6/Q5</f>
+      <c r="U6">
+        <f t="shared" ref="U6:U26" si="7">T6/T5</f>
         <v>1.0325</v>
       </c>
-      <c r="T6">
-        <f>F6/F5</f>
+      <c r="W6">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="U6">
-        <f t="shared" ref="U6:U12" si="7">T6/T5</f>
+      <c r="X6">
+        <f t="shared" ref="X6:X12" si="8">W6/W5</f>
         <v>1.05</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1883,44 +2964,47 @@
       <c r="F7" s="3">
         <v>214</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>3.3157894736842106</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="4"/>
-        <v>1.1634349030470914</v>
-      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>3.5254237288135593</v>
+        <v>3.3157894736842106</v>
       </c>
       <c r="L7">
         <f t="shared" si="5"/>
+        <v>1.1634349030470914</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>3.5254237288135593</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="6"/>
         <v>1.1950588911232403</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <f t="shared" si="0"/>
         <v>1.0288461538461537</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="3"/>
+      <c r="T7">
+        <f t="shared" si="4"/>
         <v>3.5254237288135593</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="6"/>
-        <v>1.1950588911232403</v>
-      </c>
-      <c r="T7">
-        <f>F7/F6</f>
-        <v>3.5666666666666669</v>
       </c>
       <c r="U7">
         <f t="shared" si="7"/>
+        <v>1.1950588911232403</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="1"/>
+        <v>3.5666666666666669</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="8"/>
         <v>1.1888888888888889</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1937,44 +3021,47 @@
       <c r="F8" s="3">
         <v>864</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>3.4285714285714284</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="4"/>
-        <v>1.0340136054421767</v>
-      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>3.8798076923076925</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="L8">
         <f t="shared" si="5"/>
+        <v>1.0340136054421767</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>3.8798076923076925</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="6"/>
         <v>1.1005223742603552</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <f t="shared" si="0"/>
         <v>1.0706319702602229</v>
       </c>
-      <c r="Q8">
-        <f t="shared" si="3"/>
+      <c r="T8">
+        <f t="shared" si="4"/>
         <v>3.8798076923076925</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="6"/>
-        <v>1.1005223742603552</v>
-      </c>
-      <c r="T8">
-        <f>F8/F7</f>
-        <v>4.037383177570093</v>
       </c>
       <c r="U8">
         <f t="shared" si="7"/>
+        <v>1.1005223742603552</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="1"/>
+        <v>4.037383177570093</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="8"/>
         <v>1.1319765918420821</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1991,44 +3078,47 @@
       <c r="F9" s="3">
         <v>3996</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>3.2222222222222223</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="4"/>
-        <v>0.93981481481481488</v>
-      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>4.2317224287484514</v>
+        <v>3.2222222222222223</v>
       </c>
       <c r="L9">
         <f t="shared" si="5"/>
+        <v>0.93981481481481488</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>4.2317224287484514</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
         <v>1.0907041699872093</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <f t="shared" si="0"/>
         <v>1.1701317715959005</v>
       </c>
-      <c r="Q9">
-        <f t="shared" si="3"/>
+      <c r="T9">
+        <f t="shared" si="4"/>
         <v>4.2317224287484514</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="6"/>
-        <v>1.0907041699872093</v>
-      </c>
-      <c r="T9">
-        <f>F9/F8</f>
-        <v>4.625</v>
       </c>
       <c r="U9">
         <f t="shared" si="7"/>
+        <v>1.0907041699872093</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="1"/>
+        <v>4.625</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="8"/>
         <v>1.1455439814814816</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2045,44 +3135,47 @@
       <c r="F10" s="3">
         <v>20125</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>2.7308429118773945</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>0.84750297265160512</v>
-      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>4.1991215226939973</v>
+        <v>2.7308429118773945</v>
       </c>
       <c r="L10">
         <f t="shared" si="5"/>
+        <v>0.84750297265160512</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>4.1991215226939973</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
         <v>0.99229606700265172</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <f t="shared" si="0"/>
         <v>1.4034170153417016</v>
       </c>
-      <c r="Q10">
-        <f t="shared" si="3"/>
+      <c r="T10">
+        <f t="shared" si="4"/>
         <v>4.1991215226939973</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="6"/>
-        <v>0.99229606700265172</v>
-      </c>
-      <c r="T10">
-        <f>F10/F9</f>
-        <v>5.0362862862862867</v>
       </c>
       <c r="U10">
         <f t="shared" si="7"/>
+        <v>0.99229606700265172</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="1"/>
+        <v>5.0362862862862867</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="8"/>
         <v>1.0889267646024403</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2099,43 +3192,46 @@
       <c r="F11" s="3">
         <v>105325</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>2.0464749210803226</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>0.74939313139524966</v>
-      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="K11">
         <f t="shared" si="2"/>
+        <v>2.0464749210803226</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="5"/>
+        <v>0.74939313139524966</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
         <v>3.9041841004184099</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>0.93981481481481488</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <f t="shared" si="0"/>
         <v>1.8812738899010466</v>
       </c>
-      <c r="Q11">
-        <f t="shared" si="3"/>
+      <c r="T11">
+        <f t="shared" si="4"/>
         <v>3.9041841004184099</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="6"/>
-        <v>0.92976211317495605</v>
-      </c>
-      <c r="T11">
-        <f>F11/F10</f>
-        <v>5.2335403726708076</v>
       </c>
       <c r="U11">
         <f t="shared" si="7"/>
+        <v>0.92976211317495605</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="1"/>
+        <v>5.2335403726708076</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="8"/>
         <v>1.0391665753636048</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2146,7 +3242,7 @@
         <v>188710</v>
       </c>
       <c r="D12" s="3">
-        <f>D11*K12</f>
+        <f t="shared" ref="D12:D22" si="9">D11*N12</f>
         <v>185246.90402265682</v>
       </c>
       <c r="E12" s="4">
@@ -2156,43 +3252,46 @@
       <c r="F12" s="3">
         <v>544888</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="K12">
+        <f t="shared" si="2"/>
         <v>1.3804096323592425</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
+      <c r="L12">
+        <f t="shared" si="5"/>
         <v>0.67453044165844556</v>
       </c>
-      <c r="K12">
-        <f>K11*L12</f>
+      <c r="N12">
+        <f>N11*O12</f>
         <v>3.3088076308837353</v>
       </c>
-      <c r="L12">
+      <c r="O12">
         <v>0.84750297265160512</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <f t="shared" si="0"/>
         <v>2.8874357479730803</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="3"/>
+      <c r="T12">
+        <f t="shared" si="4"/>
         <v>3.3706640945950772</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="6"/>
-        <v>0.86334660658902951</v>
-      </c>
-      <c r="T12">
-        <f>F12/F11</f>
-        <v>5.1733966294801803</v>
       </c>
       <c r="U12">
         <f t="shared" si="7"/>
+        <v>0.86334660658902951</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="1"/>
+        <v>5.1733966294801803</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="8"/>
         <v>0.98850801963720503</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2203,52 +3302,56 @@
         <v>490288</v>
       </c>
       <c r="D13" s="3">
-        <f>D12*K13</f>
+        <f t="shared" si="9"/>
         <v>459337.79931269254</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" ref="E13:E24" si="8">(C13-D13)/C13</f>
+        <f t="shared" ref="E13:E24" si="10">(C13-D13)/C13</f>
         <v>6.3126571907343151E-2</v>
       </c>
       <c r="F13" s="3">
-        <f>T14*F12</f>
+        <v>2624951</v>
+      </c>
+      <c r="G13" s="3">
         <v>2262768.1175819566</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" t="s">
         <v>3</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
+      <c r="K13">
+        <f t="shared" si="2"/>
         <v>0.82847032530419662</v>
       </c>
-      <c r="I13">
+      <c r="L13">
+        <f t="shared" si="5"/>
+        <v>0.60016266612705926</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13:N22" si="11">N12*O13</f>
+        <v>2.4795977116924597</v>
+      </c>
+      <c r="O13">
+        <v>0.74939313139524966</v>
+      </c>
+      <c r="T13">
         <f t="shared" si="4"/>
-        <v>0.60016266612705926</v>
-      </c>
-      <c r="K13">
-        <f t="shared" ref="K13:K22" si="9">K12*L13</f>
-        <v>2.4795977116924597</v>
-      </c>
-      <c r="L13">
-        <v>0.74939313139524966</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="3"/>
         <v>2.5981029092257963</v>
       </c>
-      <c r="R13">
-        <f t="shared" si="6"/>
+      <c r="U13">
+        <f t="shared" si="7"/>
         <v>0.77079852406292959</v>
       </c>
-      <c r="T13">
-        <f>T12*U13</f>
+      <c r="W13">
+        <f>W12*X13</f>
         <v>4.8100281825176872</v>
       </c>
-      <c r="U13">
+      <c r="X13">
         <v>0.92976211317495605</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2259,49 +3362,54 @@
         <v>854645</v>
       </c>
       <c r="D14" s="3">
-        <f>D13*K14</f>
+        <f t="shared" si="9"/>
         <v>768271.93109465449</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.10106309509251854</v>
       </c>
       <c r="F14" s="3">
-        <f>T15*F13</f>
+        <f t="shared" ref="F14:F27" si="12">W15*F13</f>
+        <v>8402236.1314806473</v>
+      </c>
+      <c r="G14" s="3">
         <v>7242920.7382193282</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14">
+        <f t="shared" si="2"/>
         <v>0.50640689396777816</v>
       </c>
-      <c r="I14">
+      <c r="L14">
+        <f t="shared" si="5"/>
+        <v>0.61125532019730022</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="11"/>
+        <v>1.6725641396031858</v>
+      </c>
+      <c r="O14">
+        <v>0.67453044165844556</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="4"/>
-        <v>0.61125532019730022</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="9"/>
-        <v>1.6725641396031858</v>
-      </c>
-      <c r="L14">
-        <v>0.67453044165844556</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="3"/>
         <v>1.7431489247136378</v>
       </c>
-      <c r="R14">
-        <f t="shared" si="6"/>
+      <c r="U14">
+        <f t="shared" si="7"/>
         <v>0.67093143944520484</v>
       </c>
-      <c r="T14">
-        <f t="shared" ref="T14:T28" si="10">T13*U14</f>
+      <c r="W14">
+        <f t="shared" ref="W14:W28" si="13">W13*X14</f>
         <v>4.152721508974242</v>
       </c>
-      <c r="U14">
+      <c r="X14">
         <v>0.86334660658902951</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2312,49 +3420,54 @@
         <v>914533</v>
       </c>
       <c r="D15" s="3">
-        <f>D14*K15</f>
+        <f t="shared" si="9"/>
         <v>771199.47223142162</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.15672865579326101</v>
       </c>
       <c r="F15" s="3">
-        <f>T16*F14</f>
+        <f t="shared" si="12"/>
+        <v>18044577.064273376</v>
+      </c>
+      <c r="G15" s="3">
         <v>15554840.328938868</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="K15">
+        <f t="shared" si="2"/>
         <v>0.33575022195915949</v>
       </c>
-      <c r="I15">
+      <c r="L15">
+        <f t="shared" si="5"/>
+        <v>0.66300484049200703</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="11"/>
+        <v>1.003810553292759</v>
+      </c>
+      <c r="O15">
+        <v>0.60016266612705926</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="4"/>
-        <v>0.66300484049200703</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="9"/>
-        <v>1.003810553292759</v>
-      </c>
-      <c r="L15">
-        <v>0.60016266612705926</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="3"/>
         <v>1.0700735393057936</v>
       </c>
-      <c r="R15">
-        <f t="shared" si="6"/>
+      <c r="U15">
+        <f t="shared" si="7"/>
         <v>0.61387384871982975</v>
       </c>
-      <c r="T15">
-        <f t="shared" si="10"/>
+      <c r="W15">
+        <f t="shared" si="13"/>
         <v>3.2009116099617274</v>
       </c>
-      <c r="U15">
+      <c r="X15">
         <v>0.77079852406292959</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2365,49 +3478,54 @@
         <v>607155</v>
       </c>
       <c r="D16" s="3">
-        <f>D15*K16</f>
+        <f t="shared" si="9"/>
         <v>473196.07431996724</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.22063381785546154</v>
       </c>
       <c r="F16" s="3">
-        <f>T17*F15</f>
+        <f t="shared" si="12"/>
+        <v>23789080.987431131</v>
+      </c>
+      <c r="G16" s="3">
         <v>20506734.79426254</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="K16">
+        <f t="shared" si="2"/>
         <v>0.23226090788893786</v>
       </c>
-      <c r="I16">
+      <c r="L16">
+        <f t="shared" si="5"/>
+        <v>0.69176695262822485</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="11"/>
+        <v>0.61358454117039452</v>
+      </c>
+      <c r="O16">
+        <v>0.61125532019730022</v>
+      </c>
+      <c r="T16">
         <f t="shared" si="4"/>
-        <v>0.69176695262822485</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="9"/>
-        <v>0.61358454117039452</v>
-      </c>
-      <c r="L16">
-        <v>0.61125532019730022</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="3"/>
         <v>0.66389621806976895</v>
       </c>
-      <c r="R16">
-        <f t="shared" si="6"/>
+      <c r="U16">
+        <f t="shared" si="7"/>
         <v>0.62042111470251782</v>
       </c>
-      <c r="T16">
-        <f t="shared" si="10"/>
+      <c r="W16">
+        <f t="shared" si="13"/>
         <v>2.1475922340084899</v>
       </c>
-      <c r="U16">
+      <c r="X16">
         <v>0.67093143944520484</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2418,49 +3536,54 @@
         <v>274184</v>
       </c>
       <c r="D17" s="3">
-        <f>D16*K17</f>
+        <f t="shared" si="9"/>
         <v>192500.6682608056</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.2979142901817553</v>
       </c>
       <c r="F17" s="3">
-        <f>T18*F16</f>
+        <f t="shared" si="12"/>
+        <v>19457865.272202503</v>
+      </c>
+      <c r="G17" s="3">
         <v>16773127.259954559</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="K17">
+        <f t="shared" si="2"/>
         <v>0.15370018975332067</v>
       </c>
-      <c r="I17">
+      <c r="L17">
+        <f t="shared" si="5"/>
+        <v>0.66175660445974305</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="11"/>
+        <v>0.40680952084703875</v>
+      </c>
+      <c r="O17">
+        <v>0.66300484049200703</v>
+      </c>
+      <c r="T17">
         <f t="shared" si="4"/>
-        <v>0.66175660445974305</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="9"/>
-        <v>0.40680952084703875</v>
-      </c>
-      <c r="L17">
-        <v>0.66300484049200703</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="3"/>
         <v>0.45158814470769409</v>
       </c>
-      <c r="R17">
-        <f t="shared" si="6"/>
+      <c r="U17">
+        <f t="shared" si="7"/>
         <v>0.68020894292884293</v>
       </c>
-      <c r="T17">
-        <f t="shared" si="10"/>
+      <c r="W17">
+        <f t="shared" si="13"/>
         <v>1.318350710171609</v>
       </c>
-      <c r="U17">
+      <c r="X17">
         <v>0.61387384871982975</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2471,49 +3594,54 @@
         <v>94080</v>
       </c>
       <c r="D18" s="3">
-        <f>D17*K18</f>
+        <f t="shared" si="9"/>
         <v>54173.034198483838</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.42418118411475514</v>
       </c>
       <c r="F18" s="3">
-        <f>T19*F17</f>
+        <f t="shared" si="12"/>
+        <v>10825676.786594832</v>
+      </c>
+      <c r="G18" s="3">
         <v>9331982.305175934</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="K18">
+        <f t="shared" si="2"/>
         <v>0.2839506172839506</v>
       </c>
-      <c r="I18">
+      <c r="L18">
+        <f t="shared" si="5"/>
+        <v>1.8474317939338516</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="11"/>
+        <v>0.28141738253650428</v>
+      </c>
+      <c r="O18">
+        <v>0.69176695262822485</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="4"/>
-        <v>1.8474317939338516</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="9"/>
-        <v>0.28141738253650428</v>
-      </c>
-      <c r="L18">
-        <v>0.69176695262822485</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="3"/>
         <v>0.34312724301928632</v>
       </c>
-      <c r="R18">
-        <f t="shared" si="6"/>
+      <c r="U18">
+        <f t="shared" si="7"/>
         <v>0.75982340776768442</v>
       </c>
-      <c r="T18">
-        <f t="shared" si="10"/>
+      <c r="W18">
+        <f t="shared" si="13"/>
         <v>0.81793261717352561</v>
       </c>
-      <c r="U18">
+      <c r="X18">
         <v>0.62042111470251782</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2524,49 +3652,54 @@
         <v>25783</v>
       </c>
       <c r="D19" s="3">
-        <f>D18*K19</f>
+        <f t="shared" si="9"/>
         <v>10088.633947345777</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.60870984961618979</v>
       </c>
       <c r="F19" s="3">
-        <f>T20*F18</f>
+        <f t="shared" si="12"/>
+        <v>4576438.0713549452</v>
+      </c>
+      <c r="G19" s="3">
         <v>3944994.8436943125</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="K19">
+        <f t="shared" si="2"/>
         <v>0.2608695652173913</v>
       </c>
-      <c r="I19">
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>0.91871455576559546</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="11"/>
+        <v>0.18622981150330567</v>
+      </c>
+      <c r="O19">
+        <v>0.66175660445974305</v>
+      </c>
+      <c r="T19">
         <f t="shared" si="4"/>
-        <v>0.91871455576559546</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="9"/>
-        <v>0.18622981150330567</v>
-      </c>
-      <c r="L19">
-        <v>0.66175660445974305</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="3"/>
         <v>0.27405399659863944</v>
       </c>
-      <c r="R19">
-        <f t="shared" si="6"/>
+      <c r="U19">
+        <f t="shared" si="7"/>
         <v>0.79869495114159605</v>
       </c>
-      <c r="T19">
-        <f t="shared" si="10"/>
+      <c r="W19">
+        <f t="shared" si="13"/>
         <v>0.55636508091462578</v>
       </c>
-      <c r="U19">
+      <c r="X19">
         <v>0.68020894292884293</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2577,49 +3710,54 @@
         <v>5694</v>
       </c>
       <c r="D20" s="3">
-        <f>D19*K20</f>
+        <f t="shared" si="9"/>
         <v>3470.9629800761777</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.39041746047134218</v>
       </c>
       <c r="F20" s="3">
-        <f>T21*F19</f>
+        <f t="shared" si="12"/>
+        <v>1545187.0588097367</v>
+      </c>
+      <c r="G20" s="3">
         <v>1331986.7732292558</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="K20">
+        <f t="shared" si="2"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="I20">
+      <c r="L20">
+        <f t="shared" si="5"/>
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="11"/>
+        <v>0.34404687474951501</v>
+      </c>
+      <c r="O20">
+        <v>1.8474317939338516</v>
+      </c>
+      <c r="T20">
         <f t="shared" si="4"/>
-        <v>0.63888888888888884</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="9"/>
-        <v>0.34404687474951501</v>
-      </c>
-      <c r="L20">
-        <v>1.8474317939338516</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="3"/>
         <v>0.22084319125004848</v>
       </c>
-      <c r="R20">
-        <f t="shared" si="6"/>
+      <c r="U20">
+        <f t="shared" si="7"/>
         <v>0.80583824352498012</v>
       </c>
-      <c r="T20">
-        <f t="shared" si="10"/>
+      <c r="W20">
+        <f t="shared" si="13"/>
         <v>0.42273921174349444</v>
       </c>
-      <c r="U20">
+      <c r="X20">
         <v>0.75982340776768442</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2628,41 +3766,46 @@
         <v>1106</v>
       </c>
       <c r="D21" s="3">
-        <f>D20*K21</f>
+        <f t="shared" si="9"/>
         <v>1097.1050043741125</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8.0424915243106077E-3</v>
       </c>
       <c r="F21" s="3">
-        <f>T22*F20</f>
+        <f t="shared" si="12"/>
+        <v>420419.07164462487</v>
+      </c>
+      <c r="G21" s="3">
         <v>362410.90646677278</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="9"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="N21">
+        <f t="shared" si="11"/>
         <v>0.31608087169804217</v>
       </c>
-      <c r="L21">
+      <c r="O21">
         <v>0.91871455576559546</v>
       </c>
-      <c r="Q21">
-        <f t="shared" si="3"/>
+      <c r="T21">
+        <f t="shared" si="4"/>
         <v>0.19423955040393395</v>
       </c>
-      <c r="R21">
-        <f t="shared" si="6"/>
+      <c r="U21">
+        <f t="shared" si="7"/>
         <v>0.87953606042582178</v>
       </c>
-      <c r="T21">
-        <f t="shared" si="10"/>
+      <c r="W21">
+        <f t="shared" si="13"/>
         <v>0.33763967406910711</v>
       </c>
-      <c r="U21">
+      <c r="X21">
         <v>0.79869495114159605</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2671,41 +3814,46 @@
         <v>250</v>
       </c>
       <c r="D22" s="3">
-        <f>D21*K22</f>
+        <f t="shared" si="9"/>
         <v>221.54999558104549</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.11380001767581803</v>
       </c>
       <c r="F22" s="3">
-        <f>T23*F21</f>
+        <f t="shared" si="12"/>
+        <v>100609.13277873328</v>
+      </c>
+      <c r="G22" s="3">
         <v>86727.385764262828</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="9"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="N22">
+        <f t="shared" si="11"/>
         <v>0.2019405569181936</v>
       </c>
-      <c r="L22">
+      <c r="O22">
         <v>0.63888888888888884</v>
       </c>
-      <c r="Q22">
-        <f t="shared" si="3"/>
+      <c r="T22">
+        <f t="shared" si="4"/>
         <v>0.22603978300180833</v>
       </c>
-      <c r="R22">
-        <f t="shared" si="6"/>
+      <c r="U22">
+        <f t="shared" si="7"/>
         <v>1.1637165681847168</v>
       </c>
-      <c r="T22">
-        <f t="shared" si="10"/>
+      <c r="W22">
+        <f t="shared" si="13"/>
         <v>0.27208296189619607</v>
       </c>
-      <c r="U22">
+      <c r="X22">
         <v>0.80583824352498012</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2717,30 +3865,35 @@
         <v>70</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1095890410958902E-2</v>
       </c>
       <c r="F23" s="3">
-        <f>T24*F22</f>
+        <f t="shared" si="12"/>
+        <v>28018.160559942215</v>
+      </c>
+      <c r="G23" s="3">
         <v>24152.29862512842</v>
       </c>
-      <c r="Q23">
-        <f t="shared" si="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="T23">
+        <f t="shared" si="4"/>
         <v>0.29199999999999998</v>
       </c>
-      <c r="R23">
-        <f t="shared" si="6"/>
+      <c r="U23">
+        <f t="shared" si="7"/>
         <v>1.2918079999999998</v>
       </c>
-      <c r="T23">
-        <f t="shared" si="10"/>
+      <c r="W23">
+        <f t="shared" si="13"/>
         <v>0.23930677641516929</v>
       </c>
-      <c r="U23">
+      <c r="X23">
         <v>0.87953606042582178</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2752,30 +3905,35 @@
         <v>25</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.407407407407407E-2</v>
       </c>
       <c r="F24" s="3">
-        <f>T25*F23</f>
+        <f t="shared" si="12"/>
+        <v>10079.518902591168</v>
+      </c>
+      <c r="G24" s="3">
         <v>8688.7770527327812</v>
       </c>
-      <c r="Q24">
-        <f t="shared" si="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="T24">
+        <f t="shared" si="4"/>
         <v>0.36986301369863012</v>
       </c>
-      <c r="R24">
-        <f t="shared" si="6"/>
+      <c r="U24">
+        <f t="shared" si="7"/>
         <v>1.2666541565021581</v>
       </c>
-      <c r="T24">
-        <f t="shared" si="10"/>
+      <c r="W24">
+        <f t="shared" si="13"/>
         <v>0.27848526059320811</v>
       </c>
-      <c r="U24">
+      <c r="X24">
         <v>1.1637165681847168</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2788,26 +3946,31 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3">
-        <f>T26*F24</f>
+        <f t="shared" si="12"/>
+        <v>4593.0168657211289</v>
+      </c>
+      <c r="G25" s="3">
         <v>3959.2861456347105</v>
       </c>
-      <c r="Q25">
-        <f t="shared" si="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="T25">
+        <f t="shared" si="4"/>
         <v>0.29629629629629628</v>
       </c>
-      <c r="R25">
-        <f t="shared" si="6"/>
+      <c r="U25">
+        <f t="shared" si="7"/>
         <v>0.80109739368998634</v>
       </c>
-      <c r="T25">
-        <f t="shared" si="10"/>
+      <c r="W25">
+        <f t="shared" si="13"/>
         <v>0.35974948751639091</v>
       </c>
-      <c r="U25">
+      <c r="X25">
         <v>1.2918079999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2820,43 +3983,53 @@
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3">
-        <f>T27*F25</f>
+        <f t="shared" si="12"/>
+        <v>1676.6468428181802</v>
+      </c>
+      <c r="G26" s="3">
         <v>1445.3081297035353</v>
       </c>
-      <c r="Q26">
-        <f t="shared" si="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="T26">
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
-      <c r="R26">
-        <f t="shared" si="6"/>
+      <c r="U26">
+        <f t="shared" si="7"/>
         <v>0.421875</v>
       </c>
-      <c r="T26">
-        <f t="shared" si="10"/>
+      <c r="W26">
+        <f t="shared" si="13"/>
         <v>0.45567818366215779</v>
       </c>
-      <c r="U26">
+      <c r="X26">
         <v>1.2666541565021581</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1"/>
       <c r="F27" s="3">
-        <f>T28*F26</f>
+        <f t="shared" si="12"/>
+        <v>258.20755241858529</v>
+      </c>
+      <c r="G27" s="3">
         <v>222.58084715929812</v>
       </c>
-      <c r="T27">
-        <f t="shared" si="10"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="W27">
+        <f t="shared" si="13"/>
         <v>0.36504260529314153</v>
       </c>
-      <c r="U27">
+      <c r="X27">
         <v>0.80109739368998634</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2864,15 +4037,20 @@
       <c r="F28" s="3">
         <v>50</v>
       </c>
-      <c r="T28">
-        <f t="shared" si="10"/>
+      <c r="G28" s="3">
+        <v>50</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="W28">
+        <f t="shared" si="13"/>
         <v>0.15400234910804408</v>
       </c>
-      <c r="U28">
+      <c r="X28">
         <v>0.421875</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2880,8 +4058,13 @@
       <c r="F29" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="G29" s="3">
+        <v>29</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2889,6 +4072,11 @@
       <c r="F30" s="3">
         <v>1</v>
       </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C26">
@@ -2903,7 +4091,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
+  <conditionalFormatting sqref="F2:I12 F13:F30 H13:I30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2941,4 +4129,795 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <f>B3/B2</f>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="L3">
+        <f>C3/C2</f>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <f>B4/B3</f>
+        <v>1.6</v>
+      </c>
+      <c r="J4">
+        <f>I4/I3</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L4">
+        <f>C4/C3</f>
+        <v>1.6153846153846154</v>
+      </c>
+      <c r="M4">
+        <f>L4/L3</f>
+        <v>0.74556213017751483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44</v>
+      </c>
+      <c r="I5">
+        <f>B5/B4</f>
+        <v>2.125</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J25" si="0">I5/I4</f>
+        <v>1.328125</v>
+      </c>
+      <c r="L5">
+        <f>C5/C4</f>
+        <v>2.0952380952380953</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M11" si="1">L5/L4</f>
+        <v>1.2970521541950113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1">
+        <v>102</v>
+      </c>
+      <c r="I6">
+        <f>B6/B5</f>
+        <v>1.3235294117647058</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.62283737024221453</v>
+      </c>
+      <c r="L6">
+        <f>C6/C5</f>
+        <v>2.3181818181818183</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>1.1064049586776861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>103</v>
+      </c>
+      <c r="C7" s="1">
+        <v>159</v>
+      </c>
+      <c r="I7">
+        <f>B7/B6</f>
+        <v>2.2888888888888888</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1.7293827160493827</v>
+      </c>
+      <c r="L7">
+        <f>C7/C6</f>
+        <v>1.5588235294117647</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.67243367935409448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>245</v>
+      </c>
+      <c r="C8" s="1">
+        <v>391</v>
+      </c>
+      <c r="I8">
+        <f>B8/B7</f>
+        <v>2.378640776699029</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1.0392119898199641</v>
+      </c>
+      <c r="L8">
+        <f>C8/C7</f>
+        <v>2.459119496855346</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>1.5775483564732409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1669</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3436</v>
+      </c>
+      <c r="I9">
+        <f>B9/B8</f>
+        <v>6.8122448979591841</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>2.8639233652644736</v>
+      </c>
+      <c r="L9">
+        <f>C9/C8</f>
+        <v>8.7877237851662411</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>3.5735245059883178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>15624</v>
+      </c>
+      <c r="C10" s="1">
+        <v>56887</v>
+      </c>
+      <c r="I10">
+        <f>B10/B9</f>
+        <v>9.3612941881366094</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>1.3741863847174771</v>
+      </c>
+      <c r="L10">
+        <f>C10/C9</f>
+        <v>16.556169965075668</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>1.8840111921841052</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>154239</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1237241</v>
+      </c>
+      <c r="I11">
+        <f>B11/B10</f>
+        <v>9.8719278033794158</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>1.0545473312749771</v>
+      </c>
+      <c r="L11">
+        <f>C11/C10</f>
+        <v>21.749099091180764</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>1.3136552195984514</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1062174</v>
+      </c>
+      <c r="C12" s="1">
+        <v>26637970</v>
+      </c>
+      <c r="D12" s="7">
+        <f>C12/(1000*60*60)</f>
+        <v>7.3994361111111111</v>
+      </c>
+      <c r="E12" s="7">
+        <f>D12/24</f>
+        <v>0.30830983796296296</v>
+      </c>
+      <c r="I12">
+        <f>B12/B11</f>
+        <v>6.886546204267403</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0.69758879333679491</v>
+      </c>
+      <c r="L12">
+        <f>C12/C11</f>
+        <v>21.530138428972204</v>
+      </c>
+      <c r="M12">
+        <v>0.69758879333679491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3797288</v>
+      </c>
+      <c r="C13" s="1">
+        <f>C12*L13</f>
+        <v>400080553.8246963</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" ref="D13:D24" si="2">C13/(1000*60*60)</f>
+        <v>111.13348717352675</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" ref="E13:E24" si="3">D13/24</f>
+        <v>4.6305619655636141</v>
+      </c>
+      <c r="I13">
+        <f>B13/B12</f>
+        <v>3.575015016372082</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.51913033185731672</v>
+      </c>
+      <c r="L13">
+        <f>L12*M12</f>
+        <v>15.019183287040878</v>
+      </c>
+      <c r="M13">
+        <v>0.51913033185731672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5661054</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:C29" si="4">C13*L14</f>
+        <v>3119393512.8225894</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="2"/>
+        <v>866.49819800627483</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="3"/>
+        <v>36.104091583594787</v>
+      </c>
+      <c r="I14">
+        <f>B14/B13</f>
+        <v>1.4908150237748625</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.4170094438617879</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L25" si="5">L13*M13</f>
+        <v>7.7969136040273961</v>
+      </c>
+      <c r="M14">
+        <v>0.4170094438617879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5">
+        <v>3404493</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="4"/>
+        <v>10142354285.978828</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="2"/>
+        <v>2817.3206349941188</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="3"/>
+        <v>117.38835979142162</v>
+      </c>
+      <c r="I15">
+        <f>B15/B14</f>
+        <v>0.60138854001392672</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.40339581398312113</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="5"/>
+        <v>3.251386605853873</v>
+      </c>
+      <c r="M15">
+        <v>0.40339581398312113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5">
+        <v>898401</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="4"/>
+        <v>13302668740.400059</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="2"/>
+        <v>3695.1857612222384</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="3"/>
+        <v>153.96607338425994</v>
+      </c>
+      <c r="I16">
+        <f>B16/B15</f>
+        <v>0.26388686949863022</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.43879597288721073</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="5"/>
+        <v>1.3115957464422405</v>
+      </c>
+      <c r="M16">
+        <v>0.43879597288721073</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
+        <v>126276</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="4"/>
+        <v>7655990911.5102158</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="2"/>
+        <v>2126.6641420861711</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="3"/>
+        <v>88.611005920257128</v>
+      </c>
+      <c r="I17">
+        <f>B17/B16</f>
+        <v>0.14055638851693175</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0.53263881141180214</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="5"/>
+        <v>0.57552293159485024</v>
+      </c>
+      <c r="M17">
+        <v>0.53263881141180214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5">
+        <v>12442</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="4"/>
+        <v>2346912243.2831359</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="2"/>
+        <v>651.92006757864885</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="3"/>
+        <v>27.163336149110368</v>
+      </c>
+      <c r="I18">
+        <f>B18/B17</f>
+        <v>9.8530203680826128E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0.70100124740297343</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="5"/>
+        <v>0.30654585022491693</v>
+      </c>
+      <c r="M18">
+        <v>0.70100124740297343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5">
+        <v>976</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="4"/>
+        <v>504325679.950234</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="2"/>
+        <v>140.09046665284276</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="3"/>
+        <v>5.8371027772017818</v>
+      </c>
+      <c r="I19">
+        <f>B19/B18</f>
+        <v>7.8443980067513255E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0.79614145852799423</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>0.21488902339387184</v>
+      </c>
+      <c r="M19">
+        <v>0.79614145852799423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5">
+        <v>68</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="4"/>
+        <v>86281076.492204174</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="2"/>
+        <v>23.966965692278936</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="3"/>
+        <v>0.99862357051162232</v>
+      </c>
+      <c r="I20">
+        <f>B20/B19</f>
+        <v>6.9672131147540978E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0.88817690137059935</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="5"/>
+        <v>0.17108206050645339</v>
+      </c>
+      <c r="M20">
+        <v>0.88817690137059935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="4"/>
+        <v>13110507.448580027</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="2"/>
+        <v>3.6418076246055628</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="3"/>
+        <v>0.15174198435856512</v>
+      </c>
+      <c r="I21">
+        <f>B21/B20</f>
+        <v>0.14705882352941177</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>2.1107266435986163</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="5"/>
+        <v>0.15195113438071917</v>
+      </c>
+      <c r="M21">
+        <v>2.1107266435986163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="4"/>
+        <v>4204897.7586932462</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1680271551925683</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="3"/>
+        <v>4.8667798133023681E-2</v>
+      </c>
+      <c r="I22">
+        <f>B22/B21</f>
+        <v>0.3</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="5"/>
+        <v>0.32072730786241765</v>
+      </c>
+      <c r="M22">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="4"/>
+        <v>2751196.0974840932</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="2"/>
+        <v>0.76422113819002591</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="3"/>
+        <v>3.1842547424584415E-2</v>
+      </c>
+      <c r="I23">
+        <f>B23/B22</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="5"/>
+        <v>0.654283708039332</v>
+      </c>
+      <c r="M23">
+        <v>1.1111111111111112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="4"/>
+        <v>2000069.7602280357</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="2"/>
+        <v>0.55557493339667663</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="3"/>
+        <v>2.3148955558194861E-2</v>
+      </c>
+      <c r="I24">
+        <f>B24/B23</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="5"/>
+        <v>0.72698189782148004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I25" t="e">
+        <f>B25/B24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J25" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>